<commit_message>
new codes for Jenkins CICD
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Batch13ExcelFile.xlsx
+++ b/src/test/resources/testData/Batch13ExcelFile.xlsx
@@ -49,7 +49,7 @@
     <t>C:\Users\Nnoor\OneDrive\Desktop\imagefromgoogle.jpg</t>
   </si>
   <si>
-    <t>ahskljdhja231</t>
+    <t>ahskljdhja2312</t>
   </si>
   <si>
     <t>Syntax123!</t>
@@ -58,13 +58,13 @@
     <t>maks89</t>
   </si>
   <si>
-    <t>lakjsdkl89</t>
+    <t>dsfsdf21</t>
   </si>
   <si>
     <t>maks90</t>
   </si>
   <si>
-    <t>kljahsklde89798</t>
+    <t>sdfsdfsd4</t>
   </si>
 </sst>
 </file>
@@ -72,10 +72,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -86,20 +86,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,45 +102,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -200,29 +186,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -239,25 +239,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -269,19 +377,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,49 +401,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,79 +419,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,32 +433,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,22 +501,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,148 +535,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
new headless browsing codes for Jenkins CICD
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Batch13ExcelFile.xlsx
+++ b/src/test/resources/testData/Batch13ExcelFile.xlsx
@@ -49,7 +49,7 @@
     <t>C:\Users\Nnoor\OneDrive\Desktop\imagefromgoogle.jpg</t>
   </si>
   <si>
-    <t>ahskljdhja2312</t>
+    <t>sdfsdfs45</t>
   </si>
   <si>
     <t>Syntax123!</t>
@@ -58,13 +58,13 @@
     <t>maks89</t>
   </si>
   <si>
-    <t>dsfsdf21</t>
+    <t>sdfsdf564</t>
   </si>
   <si>
     <t>maks90</t>
   </si>
   <si>
-    <t>sdfsdfsd4</t>
+    <t>gdfg546</t>
   </si>
 </sst>
 </file>
@@ -73,8 +73,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -86,9 +86,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -96,22 +95,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -124,24 +130,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -155,8 +145,54 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -186,42 +222,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -239,13 +239,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -257,169 +401,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -435,10 +435,43 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
       <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -468,15 +501,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -488,30 +512,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -535,148 +535,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1006,7 +1006,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="6"/>

</xml_diff>